<commit_message>
Major change on Arduino folder
* Changed Works_017 and Works_018 into four parts
* Updated theme color
+ Added folder for instructor use
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
   <si>
     <t>List of Components</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Practical Example: Rotary Encoder</t>
   </si>
   <si>
-    <t>Summerizing Build: 4-bit Calculator</t>
-  </si>
-  <si>
     <t>Issued</t>
   </si>
   <si>
@@ -263,12 +260,6 @@
     <t>Exercise 002: Button Matrix</t>
   </si>
   <si>
-    <t>Exercise 003: Fading While Moving</t>
-  </si>
-  <si>
-    <t>Exercise 004: Do-It-Yourself</t>
-  </si>
-  <si>
     <t>Basic Structure of Python</t>
   </si>
   <si>
@@ -288,6 +279,30 @@
   </si>
   <si>
     <t>Practical Example: IoT</t>
+  </si>
+  <si>
+    <t>17-a</t>
+  </si>
+  <si>
+    <t>17-b</t>
+  </si>
+  <si>
+    <t>18-a</t>
+  </si>
+  <si>
+    <t>18-b</t>
+  </si>
+  <si>
+    <t>SPI Communication: Micro SD Card</t>
+  </si>
+  <si>
+    <t>Exercise 003: Do-It-Yourself</t>
+  </si>
+  <si>
+    <t>Exercise 004: Fading While Moving</t>
+  </si>
+  <si>
+    <t>Arduino: Bootloader</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1442,7 @@
     </row>
     <row r="17" spans="2:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3">
         <v>4</v>
@@ -1590,10 +1605,10 @@
         <v>5</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>12</v>
@@ -1867,7 +1882,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="3">
         <v>4</v>
@@ -2028,10 +2043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D55"/>
+  <dimension ref="B1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -2049,13 +2064,13 @@
     <row r="1" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2063,7 +2078,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="17">
         <v>0</v>
@@ -2225,7 +2240,7 @@
         <v>30</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D19" s="14">
         <v>10</v>
@@ -2276,7 +2291,7 @@
         <v>30</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D24" s="14">
         <v>12</v>
@@ -2287,7 +2302,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D25" s="25">
         <v>13</v>
@@ -2298,7 +2313,7 @@
         <v>31</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="13">
         <v>0</v>
@@ -2309,7 +2324,7 @@
         <v>31</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D27" s="14">
         <v>1</v>
@@ -2320,7 +2335,7 @@
         <v>31</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D28" s="14">
         <v>2</v>
@@ -2331,7 +2346,7 @@
         <v>31</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D29" s="14">
         <v>3</v>
@@ -2342,7 +2357,7 @@
         <v>31</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="14">
         <v>4</v>
@@ -2353,7 +2368,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D31" s="14"/>
     </row>
@@ -2362,7 +2377,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="14">
         <v>5</v>
@@ -2373,7 +2388,7 @@
         <v>31</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D33" s="14">
         <v>6</v>
@@ -2384,7 +2399,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D34" s="14"/>
     </row>
@@ -2415,7 +2430,7 @@
         <v>31</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="14"/>
     </row>
@@ -2426,8 +2441,8 @@
       <c r="C38" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="14">
-        <v>17</v>
+      <c r="D38" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -2435,10 +2450,10 @@
         <v>31</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="14">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -2446,21 +2461,21 @@
         <v>31</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="14">
-        <v>9</v>
+        <v>55</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="14">
-        <v>10</v>
+      <c r="C41" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -2468,20 +2483,22 @@
         <v>31</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="D42" s="14">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" s="14"/>
+      <c r="C43" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="14">
+        <v>23</v>
+      </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
@@ -2543,7 +2560,7 @@
         <v>31</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D49" s="14"/>
     </row>
@@ -2552,10 +2569,10 @@
         <v>31</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="D50" s="14">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
@@ -2563,10 +2580,10 @@
         <v>31</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="D51" s="14">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
@@ -2574,18 +2591,18 @@
         <v>31</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D52" s="14">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="23" t="s">
-        <v>66</v>
+      <c r="C53" s="21" t="s">
+        <v>94</v>
       </c>
       <c r="D53" s="14"/>
     </row>
@@ -2593,19 +2610,61 @@
       <c r="B54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C54" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="14"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="14"/>
-    </row>
-    <row r="55" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C55" s="24" t="s">
+      <c r="D58" s="14"/>
+    </row>
+    <row r="59" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="15"/>
+      <c r="D59" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more works for 017
* Moved 017_b to 017_c
+ Added 017_b for how to start with Arduino Wire Library
* Updated Workshop plan
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie Shin\Desktop\~\CS\Repositories\Workshop_Materials\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
@@ -10,12 +15,12 @@
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
     <sheet name="Workshop List" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="97">
   <si>
     <t>List of Components</t>
   </si>
@@ -303,12 +308,15 @@
   </si>
   <si>
     <t>Arduino: Bootloader</t>
+  </si>
+  <si>
+    <t>17-c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -836,6 +844,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -883,7 +894,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -916,9 +927,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -951,6 +979,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2043,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D59"/>
+  <dimension ref="B1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -2461,32 +2506,32 @@
         <v>31</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="20" t="s">
         <v>55</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="14">
-        <v>22</v>
+      <c r="C42" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -2494,10 +2539,10 @@
         <v>31</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="D43" s="14">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -2505,10 +2550,10 @@
         <v>31</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D44" s="14">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -2516,10 +2561,10 @@
         <v>31</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D45" s="14">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -2527,10 +2572,10 @@
         <v>31</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D46" s="14">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -2538,10 +2583,10 @@
         <v>31</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D47" s="14">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -2549,41 +2594,41 @@
         <v>31</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" s="14">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="14"/>
+      <c r="C49" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="14">
+        <v>16</v>
+      </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" s="14">
-        <v>9</v>
-      </c>
+      <c r="C50" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="14"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D51" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
@@ -2591,41 +2636,41 @@
         <v>31</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D52" s="14">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="D53" s="14"/>
+      <c r="C53" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="14">
+        <v>11</v>
+      </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D54" s="14">
-        <v>19</v>
-      </c>
+      <c r="C54" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D55" s="14">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
@@ -2633,38 +2678,49 @@
         <v>31</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D56" s="14">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="14"/>
+      <c r="C57" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="14">
+        <v>21</v>
+      </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D58" s="14"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D58" s="14"/>
-    </row>
-    <row r="59" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" s="24" t="s">
+      <c r="D59" s="14"/>
+    </row>
+    <row r="60" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="15"/>
+      <c r="D60" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed files to C89 Standard
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -783,6 +783,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -801,7 +804,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -811,12 +817,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1160,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1177,13 +1177,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -1213,7 +1213,7 @@
         <v>2.57</v>
       </c>
       <c r="E4" s="4">
-        <f>D4*C4</f>
+        <f t="shared" ref="E4:E18" si="0">D4*C4</f>
         <v>2.57</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -1231,7 +1231,7 @@
         <v>0.76</v>
       </c>
       <c r="E5" s="4">
-        <f>D5*C5</f>
+        <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -1249,7 +1249,7 @@
         <v>0.21</v>
       </c>
       <c r="E6" s="4">
-        <f>D6*C6</f>
+        <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -1267,7 +1267,7 @@
         <v>0.1</v>
       </c>
       <c r="E7" s="4">
-        <f>D7*C7</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -1285,7 +1285,7 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="4">
-        <f>D8*C8</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -1303,7 +1303,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="E9" s="4">
-        <f>D9*C9</f>
+        <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="F9" s="6" t="s">
@@ -1321,7 +1321,7 @@
         <v>0.39</v>
       </c>
       <c r="E10" s="4">
-        <f>D10*C10</f>
+        <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -1339,7 +1339,7 @@
         <v>0.46</v>
       </c>
       <c r="E11" s="4">
-        <f>D11*C11</f>
+        <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
       <c r="F11" s="6" t="s">
@@ -1357,7 +1357,7 @@
         <v>0.46</v>
       </c>
       <c r="E12" s="4">
-        <f>D12*C12</f>
+        <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -1375,7 +1375,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="E13" s="4">
-        <f>D13*C13</f>
+        <f t="shared" si="0"/>
         <v>1.02</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1393,7 +1393,7 @@
         <v>0.81</v>
       </c>
       <c r="E14" s="4">
-        <f>D14*C14</f>
+        <f t="shared" si="0"/>
         <v>0.81</v>
       </c>
       <c r="F14" s="6" t="s">
@@ -1411,7 +1411,7 @@
         <v>0.1</v>
       </c>
       <c r="E15" s="4">
-        <f>D15*C15</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F15" s="6" t="s">
@@ -1429,7 +1429,7 @@
         <v>4.95</v>
       </c>
       <c r="E16" s="4">
-        <f>D16*C16</f>
+        <f t="shared" si="0"/>
         <v>4.95</v>
       </c>
       <c r="F16" s="6" t="s">
@@ -1447,7 +1447,7 @@
         <v>5.95</v>
       </c>
       <c r="E17" s="4">
-        <f>D17*C17</f>
+        <f t="shared" si="0"/>
         <v>11.9</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1465,7 +1465,7 @@
         <v>1.95</v>
       </c>
       <c r="E18" s="4">
-        <f>D18*C18</f>
+        <f t="shared" si="0"/>
         <v>5.85</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -1473,11 +1473,11 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="7">
         <f>SUM(E4:E18)</f>
         <v>32.380000000000003</v>
@@ -1485,13 +1485,13 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -2051,10 +2051,10 @@
         <v>24</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D43" s="14">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
@@ -2062,10 +2062,10 @@
         <v>24</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D44" s="14">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -2073,10 +2073,10 @@
         <v>24</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D45" s="14">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -2084,10 +2084,10 @@
         <v>24</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D46" s="14">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
@@ -2095,42 +2095,42 @@
         <v>24</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D47" s="14">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="14">
-        <v>15</v>
-      </c>
+      <c r="C48" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D49" s="14">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D50" s="14"/>
+      <c r="C50" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="14">
+        <v>23</v>
+      </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
@@ -2229,7 +2229,7 @@
       <c r="B60" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="33" t="s">
+      <c r="C60" s="27" t="s">
         <v>85</v>
       </c>
       <c r="D60" s="15"/>

</xml_diff>